<commit_message>
update fiche de temps tj HO contention
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F6D109-4B66-0B4B-A2C9-6DA8EF499BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419EE748-829C-5745-9274-33EE24A24423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="tXIlrKoF4sl/1pPObgUAUr8/9fTwsaKKRyp30Qnf3LFl7mpRUflzIeDJFe4q5xuivbNmzhnFZAxmYbG92AoamA==" workbookSaltValue="oLmK1PdAPfyEkYmQkQ28Ng==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille de temps" sheetId="8" r:id="rId1"/>
@@ -835,9 +835,6 @@
     <t>5.2.</t>
   </si>
   <si>
-    <t>HOSPITALISATIONS SOUS CONTRAINTE</t>
-  </si>
-  <si>
     <t>5.3.</t>
   </si>
   <si>
@@ -1421,6 +1418,9 @@
   </si>
   <si>
     <t>Temps partiel</t>
+  </si>
+  <si>
+    <t>HO - CONTENTION</t>
   </si>
 </sst>
 </file>
@@ -2278,16 +2278,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="13" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="13" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2306,6 +2300,12 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -4496,12 +4496,12 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="121"/>
-      <c r="B6" s="157" t="s">
+      <c r="B6" s="155" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="157"/>
-      <c r="D6" s="157"/>
-      <c r="E6" s="158"/>
+      <c r="C6" s="155"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="156"/>
       <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:7" ht="110" customHeight="1" thickTop="1">
@@ -4526,8 +4526,8 @@
       <c r="B8" s="130" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="159"/>
-      <c r="D8" s="160"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="158"/>
       <c r="E8" s="131" t="s">
         <v>90</v>
       </c>
@@ -4537,7 +4537,7 @@
       <c r="A9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="161" t="s">
+      <c r="B9" s="159" t="s">
         <v>92</v>
       </c>
       <c r="C9" s="132" t="s">
@@ -4551,7 +4551,7 @@
       <c r="A10" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="161"/>
+      <c r="B10" s="159"/>
       <c r="C10" s="132" t="s">
         <v>95</v>
       </c>
@@ -4563,7 +4563,7 @@
       <c r="A11" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="161"/>
+      <c r="B11" s="159"/>
       <c r="C11" s="132" t="s">
         <v>97</v>
       </c>
@@ -4575,7 +4575,7 @@
       <c r="A12" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="161"/>
+      <c r="B12" s="159"/>
       <c r="C12" s="132" t="s">
         <v>99</v>
       </c>
@@ -4602,7 +4602,7 @@
       <c r="A14" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="153" t="s">
         <v>103</v>
       </c>
       <c r="C14" s="132" t="s">
@@ -4727,7 +4727,7 @@
       <c r="A24" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="156" t="s">
+      <c r="B24" s="153" t="s">
         <v>124</v>
       </c>
       <c r="C24" s="132" t="s">
@@ -4840,7 +4840,7 @@
       <c r="A33" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="156" t="s">
+      <c r="B33" s="153" t="s">
         <v>142</v>
       </c>
       <c r="C33" s="132" t="s">
@@ -5085,7 +5085,7 @@
       <c r="A53" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="B53" s="153" t="s">
+      <c r="B53" s="160" t="s">
         <v>183</v>
       </c>
       <c r="C53" s="132" t="s">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="B54" s="154"/>
       <c r="C54" s="132" t="s">
-        <v>186</v>
+        <v>381</v>
       </c>
       <c r="D54" s="132"/>
       <c r="E54" s="133"/>
@@ -5109,11 +5109,11 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B55" s="154"/>
       <c r="C55" s="132" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D55" s="132"/>
       <c r="E55" s="133"/>
@@ -5121,10 +5121,10 @@
     </row>
     <row r="56" spans="1:6" ht="32" customHeight="1" thickBot="1">
       <c r="A56" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56" s="139" t="s">
         <v>189</v>
-      </c>
-      <c r="B56" s="139" t="s">
-        <v>190</v>
       </c>
       <c r="C56" s="135"/>
       <c r="D56" s="135"/>
@@ -5136,13 +5136,13 @@
     </row>
     <row r="57" spans="1:6" ht="16" thickTop="1">
       <c r="A57" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57" s="153" t="s">
         <v>191</v>
       </c>
-      <c r="B57" s="156" t="s">
+      <c r="C57" s="132" t="s">
         <v>192</v>
-      </c>
-      <c r="C57" s="132" t="s">
-        <v>193</v>
       </c>
       <c r="D57" s="132"/>
       <c r="E57" s="133"/>
@@ -5150,11 +5150,11 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B58" s="154"/>
       <c r="C58" s="132" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D58" s="132"/>
       <c r="E58" s="133"/>
@@ -5162,10 +5162,10 @@
     </row>
     <row r="59" spans="1:6" ht="27" customHeight="1" thickBot="1">
       <c r="A59" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" s="138" t="s">
         <v>196</v>
-      </c>
-      <c r="B59" s="138" t="s">
-        <v>197</v>
       </c>
       <c r="C59" s="135"/>
       <c r="D59" s="135"/>
@@ -5177,13 +5177,13 @@
     </row>
     <row r="60" spans="1:6" ht="16" thickTop="1">
       <c r="A60" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B60" s="153" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="156" t="s">
+      <c r="C60" s="132" t="s">
         <v>199</v>
-      </c>
-      <c r="C60" s="132" t="s">
-        <v>200</v>
       </c>
       <c r="D60" s="132"/>
       <c r="E60" s="133"/>
@@ -5191,11 +5191,11 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B61" s="154"/>
       <c r="C61" s="132" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D61" s="132"/>
       <c r="E61" s="133"/>
@@ -5203,11 +5203,11 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B62" s="154"/>
       <c r="C62" s="132" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D62" s="132"/>
       <c r="E62" s="133"/>
@@ -5215,11 +5215,11 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B63" s="154"/>
       <c r="C63" s="132" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D63" s="132"/>
       <c r="E63" s="133"/>
@@ -5227,11 +5227,11 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B64" s="154"/>
       <c r="C64" s="132" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D64" s="132"/>
       <c r="E64" s="133"/>
@@ -5239,11 +5239,11 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B65" s="154"/>
       <c r="C65" s="132" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D65" s="132"/>
       <c r="E65" s="133"/>
@@ -5251,11 +5251,11 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B66" s="154"/>
       <c r="C66" s="132" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D66" s="132"/>
       <c r="E66" s="133"/>
@@ -5263,11 +5263,11 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B67" s="154"/>
       <c r="C67" s="132" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D67" s="132"/>
       <c r="E67" s="133"/>
@@ -5275,11 +5275,11 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B68" s="154"/>
       <c r="C68" s="132" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D68" s="132"/>
       <c r="E68" s="133"/>
@@ -5287,11 +5287,11 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B69" s="154"/>
       <c r="C69" s="132" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D69" s="132"/>
       <c r="E69" s="133"/>
@@ -5299,11 +5299,11 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B70" s="154"/>
       <c r="C70" s="132" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D70" s="132"/>
       <c r="E70" s="133"/>
@@ -5311,11 +5311,11 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B71" s="154"/>
       <c r="C71" s="132" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D71" s="132"/>
       <c r="E71" s="133"/>
@@ -5323,11 +5323,11 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B72" s="154"/>
       <c r="C72" s="132" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D72" s="132"/>
       <c r="E72" s="133"/>
@@ -5335,11 +5335,11 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B73" s="154"/>
       <c r="C73" s="132" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D73" s="132"/>
       <c r="E73" s="133"/>
@@ -5347,11 +5347,11 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B74" s="154"/>
       <c r="C74" s="132" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D74" s="132"/>
       <c r="E74" s="133"/>
@@ -5359,11 +5359,11 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B75" s="154"/>
       <c r="C75" s="132" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D75" s="132"/>
       <c r="E75" s="133"/>
@@ -5371,10 +5371,10 @@
     </row>
     <row r="76" spans="1:6" ht="35" customHeight="1" thickBot="1">
       <c r="A76" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B76" s="138" t="s">
         <v>231</v>
-      </c>
-      <c r="B76" s="138" t="s">
-        <v>232</v>
       </c>
       <c r="C76" s="135"/>
       <c r="D76" s="135"/>
@@ -5386,13 +5386,13 @@
     </row>
     <row r="77" spans="1:6" ht="16" thickTop="1">
       <c r="A77" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" s="160" t="s">
         <v>233</v>
       </c>
-      <c r="B77" s="153" t="s">
+      <c r="C77" s="132" t="s">
         <v>234</v>
-      </c>
-      <c r="C77" s="132" t="s">
-        <v>235</v>
       </c>
       <c r="D77" s="132"/>
       <c r="E77" s="133"/>
@@ -5400,11 +5400,11 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B78" s="154"/>
       <c r="C78" s="132" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D78" s="132"/>
       <c r="E78" s="133"/>
@@ -5412,11 +5412,11 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B79" s="154"/>
       <c r="C79" s="132" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D79" s="132"/>
       <c r="E79" s="133"/>
@@ -5424,11 +5424,11 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B80" s="154"/>
       <c r="C80" s="132" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D80" s="132"/>
       <c r="E80" s="133"/>
@@ -5436,11 +5436,11 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B81" s="154"/>
       <c r="C81" s="132" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D81" s="132"/>
       <c r="E81" s="133"/>
@@ -5448,10 +5448,10 @@
     </row>
     <row r="82" spans="1:6" ht="38" customHeight="1" thickBot="1">
       <c r="A82" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B82" s="138" t="s">
         <v>244</v>
-      </c>
-      <c r="B82" s="138" t="s">
-        <v>245</v>
       </c>
       <c r="C82" s="135"/>
       <c r="D82" s="135"/>
@@ -5463,13 +5463,13 @@
     </row>
     <row r="83" spans="1:6" ht="16" thickTop="1">
       <c r="A83" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B83" s="160" t="s">
         <v>246</v>
       </c>
-      <c r="B83" s="153" t="s">
+      <c r="C83" s="132" t="s">
         <v>247</v>
-      </c>
-      <c r="C83" s="132" t="s">
-        <v>248</v>
       </c>
       <c r="D83" s="132"/>
       <c r="E83" s="140"/>
@@ -5477,11 +5477,11 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B84" s="154"/>
       <c r="C84" s="132" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D84" s="132"/>
       <c r="E84" s="140"/>
@@ -5489,11 +5489,11 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B85" s="154"/>
       <c r="C85" s="132" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D85" s="132"/>
       <c r="E85" s="140"/>
@@ -5501,11 +5501,11 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B86" s="154"/>
       <c r="C86" s="132" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D86" s="132"/>
       <c r="E86" s="140"/>
@@ -5513,10 +5513,10 @@
     </row>
     <row r="87" spans="1:6" ht="26" customHeight="1" thickBot="1">
       <c r="A87" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B87" s="138" t="s">
         <v>255</v>
-      </c>
-      <c r="B87" s="138" t="s">
-        <v>256</v>
       </c>
       <c r="C87" s="135"/>
       <c r="D87" s="135"/>
@@ -5528,13 +5528,13 @@
     </row>
     <row r="88" spans="1:6" ht="16" thickTop="1">
       <c r="A88" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B88" s="160" t="s">
         <v>257</v>
       </c>
-      <c r="B88" s="153" t="s">
+      <c r="C88" s="132" t="s">
         <v>258</v>
-      </c>
-      <c r="C88" s="132" t="s">
-        <v>259</v>
       </c>
       <c r="D88" s="132"/>
       <c r="E88" s="133"/>
@@ -5542,11 +5542,11 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B89" s="154"/>
       <c r="C89" s="132" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D89" s="132"/>
       <c r="E89" s="133"/>
@@ -5554,10 +5554,10 @@
     </row>
     <row r="90" spans="1:6" ht="28" customHeight="1" thickBot="1">
       <c r="A90" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B90" s="138" t="s">
         <v>262</v>
-      </c>
-      <c r="B90" s="138" t="s">
-        <v>263</v>
       </c>
       <c r="C90" s="135"/>
       <c r="D90" s="135"/>
@@ -5569,13 +5569,13 @@
     </row>
     <row r="91" spans="1:6" ht="16" thickTop="1">
       <c r="A91" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="B91" s="160" t="s">
         <v>264</v>
       </c>
-      <c r="B91" s="153" t="s">
+      <c r="C91" s="132" t="s">
         <v>265</v>
-      </c>
-      <c r="C91" s="132" t="s">
-        <v>266</v>
       </c>
       <c r="D91" s="132"/>
       <c r="E91" s="133"/>
@@ -5583,11 +5583,11 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B92" s="154"/>
       <c r="C92" s="132" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D92" s="132"/>
       <c r="E92" s="133"/>
@@ -5595,11 +5595,11 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B93" s="154"/>
       <c r="C93" s="132" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D93" s="132"/>
       <c r="E93" s="133"/>
@@ -5607,11 +5607,11 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B94" s="154"/>
       <c r="C94" s="132" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D94" s="132"/>
       <c r="E94" s="133"/>
@@ -5619,11 +5619,11 @@
     </row>
     <row r="95" spans="1:6" s="152" customFormat="1">
       <c r="A95" s="148" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B95" s="154"/>
       <c r="C95" s="149" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D95" s="149"/>
       <c r="E95" s="150"/>
@@ -5631,11 +5631,11 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B96" s="154"/>
       <c r="C96" s="132" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D96" s="132"/>
       <c r="E96" s="133"/>
@@ -5643,11 +5643,11 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B97" s="154"/>
       <c r="C97" s="132" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D97" s="132"/>
       <c r="E97" s="133"/>
@@ -5657,7 +5657,7 @@
       <c r="A98" s="10"/>
       <c r="B98" s="137"/>
       <c r="C98" s="132" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D98" s="132"/>
       <c r="E98" s="133"/>
@@ -5667,7 +5667,7 @@
       <c r="A99" s="10"/>
       <c r="B99" s="137"/>
       <c r="C99" s="132" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D99" s="132"/>
       <c r="E99" s="133"/>
@@ -5677,7 +5677,7 @@
       <c r="A100" s="10"/>
       <c r="B100" s="137"/>
       <c r="C100" s="132" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D100" s="132"/>
       <c r="E100" s="133"/>
@@ -5686,19 +5686,19 @@
     <row r="101" spans="1:6">
       <c r="A101" s="10"/>
       <c r="B101" s="137"/>
-      <c r="C101" s="155" t="s">
-        <v>282</v>
-      </c>
-      <c r="D101" s="155"/>
+      <c r="C101" s="161" t="s">
+        <v>281</v>
+      </c>
+      <c r="D101" s="161"/>
       <c r="E101" s="133"/>
       <c r="F101" s="42"/>
     </row>
     <row r="102" spans="1:6" ht="23" customHeight="1" thickBot="1">
       <c r="A102" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B102" s="138" t="s">
         <v>283</v>
-      </c>
-      <c r="B102" s="138" t="s">
-        <v>284</v>
       </c>
       <c r="C102" s="135"/>
       <c r="D102" s="135"/>
@@ -5729,15 +5729,9 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="oZ4bML4lPRSuNDzzgWiF5qBK4aygiW2FWBscJrI5fOYxicE2NxR8/QXKyCe4YR0YZAfB2EB03Cib7FNjng35/A==" saltValue="QPN4XZnrjgrszjXG9G6XKQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="tVZa7NABdsRO2B2x23XDKOK2hNT5bA2qWv3gJEEjUVsInyHE2VaMzOLtqCtO6gacq+4UUdOpllgUV75YZbnQ9w==" saltValue="lqJ/fIOWMHEWw4k4z+ihgA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="14">
-    <mergeCell ref="B33:B51"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B14:B22"/>
-    <mergeCell ref="B24:B31"/>
     <mergeCell ref="B91:B97"/>
     <mergeCell ref="C101:D101"/>
     <mergeCell ref="B53:B55"/>
@@ -5746,6 +5740,12 @@
     <mergeCell ref="B77:B81"/>
     <mergeCell ref="B83:B86"/>
     <mergeCell ref="B88:B89"/>
+    <mergeCell ref="B33:B51"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B14:B22"/>
+    <mergeCell ref="B24:B31"/>
   </mergeCells>
   <conditionalFormatting sqref="B23">
     <cfRule type="expression" dxfId="13" priority="17">
@@ -5866,32 +5866,32 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="144" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="144" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="144" t="s">
+      <c r="C1" s="145" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="145" t="s">
-        <v>287</v>
-      </c>
       <c r="E1" s="144" t="s">
+        <v>284</v>
+      </c>
+      <c r="F1" s="144" t="s">
         <v>285</v>
       </c>
-      <c r="F1" s="144" t="s">
+      <c r="G1" s="145" t="s">
         <v>286</v>
-      </c>
-      <c r="G1" s="145" t="s">
-        <v>287</v>
       </c>
       <c r="H1" s="145"/>
       <c r="I1" s="144" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1" s="144" t="s">
         <v>285</v>
       </c>
-      <c r="J1" s="144" t="s">
+      <c r="K1" s="145" t="s">
         <v>286</v>
-      </c>
-      <c r="K1" s="145" t="s">
-        <v>287</v>
       </c>
       <c r="M1" t="s">
         <v>50</v>
@@ -5899,92 +5899,92 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" t="s">
         <v>288</v>
-      </c>
-      <c r="B2" t="s">
-        <v>289</v>
       </c>
       <c r="C2" s="146">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G2" s="147">
         <v>2</v>
       </c>
       <c r="I2" t="s">
+        <v>290</v>
+      </c>
+      <c r="J2" t="s">
         <v>291</v>
-      </c>
-      <c r="J2" t="s">
-        <v>292</v>
       </c>
       <c r="K2">
         <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B3" t="s">
         <v>294</v>
-      </c>
-      <c r="B3" t="s">
-        <v>295</v>
       </c>
       <c r="C3" s="146">
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F3" t="s">
         <v>296</v>
-      </c>
-      <c r="F3" t="s">
-        <v>297</v>
       </c>
       <c r="G3" s="147">
         <v>2</v>
       </c>
       <c r="I3" t="s">
+        <v>297</v>
+      </c>
+      <c r="J3" t="s">
         <v>298</v>
-      </c>
-      <c r="J3" t="s">
-        <v>299</v>
       </c>
       <c r="K3">
         <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" t="s">
         <v>301</v>
-      </c>
-      <c r="B4" t="s">
-        <v>302</v>
       </c>
       <c r="C4" s="146">
         <v>1</v>
       </c>
       <c r="E4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F4" t="s">
         <v>303</v>
-      </c>
-      <c r="F4" t="s">
-        <v>304</v>
       </c>
       <c r="G4" s="147">
         <v>2</v>
       </c>
       <c r="I4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J4" t="s">
         <v>305</v>
-      </c>
-      <c r="J4" t="s">
-        <v>306</v>
       </c>
       <c r="K4">
         <v>3</v>
@@ -5992,28 +5992,28 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5" t="s">
         <v>307</v>
-      </c>
-      <c r="B5" t="s">
-        <v>308</v>
       </c>
       <c r="C5" s="146">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G5" s="147">
         <v>2</v>
       </c>
       <c r="I5" t="s">
+        <v>309</v>
+      </c>
+      <c r="J5" t="s">
         <v>310</v>
-      </c>
-      <c r="J5" t="s">
-        <v>311</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -6021,25 +6021,25 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B6" t="s">
         <v>312</v>
-      </c>
-      <c r="B6" t="s">
-        <v>313</v>
       </c>
       <c r="C6" s="146">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G6" s="147">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -6047,25 +6047,25 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
+        <v>315</v>
+      </c>
+      <c r="B7" t="s">
         <v>316</v>
-      </c>
-      <c r="B7" t="s">
-        <v>317</v>
       </c>
       <c r="C7" s="146">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G7" s="147">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K7">
         <v>3</v>
@@ -6073,25 +6073,25 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B8" t="s">
         <v>320</v>
-      </c>
-      <c r="B8" t="s">
-        <v>321</v>
       </c>
       <c r="C8" s="146">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G8" s="147">
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K8">
         <v>3</v>
@@ -6099,19 +6099,19 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
+        <v>322</v>
+      </c>
+      <c r="B9" t="s">
         <v>323</v>
-      </c>
-      <c r="B9" t="s">
-        <v>324</v>
       </c>
       <c r="C9" s="146">
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>324</v>
+      </c>
+      <c r="F9" t="s">
         <v>325</v>
-      </c>
-      <c r="F9" t="s">
-        <v>326</v>
       </c>
       <c r="G9" s="147">
         <v>2</v>
@@ -6119,19 +6119,19 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
+        <v>326</v>
+      </c>
+      <c r="B10" t="s">
         <v>327</v>
-      </c>
-      <c r="B10" t="s">
-        <v>328</v>
       </c>
       <c r="C10" s="146">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G10" s="147">
         <v>2</v>
@@ -6139,19 +6139,19 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
+        <v>329</v>
+      </c>
+      <c r="B11" t="s">
         <v>330</v>
-      </c>
-      <c r="B11" t="s">
-        <v>331</v>
       </c>
       <c r="C11" s="146">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G11" s="147">
         <v>2</v>
@@ -6159,19 +6159,19 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
+        <v>332</v>
+      </c>
+      <c r="B12" t="s">
         <v>333</v>
-      </c>
-      <c r="B12" t="s">
-        <v>334</v>
       </c>
       <c r="C12" s="146">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G12" s="147">
         <v>2</v>
@@ -6179,19 +6179,19 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
+        <v>335</v>
+      </c>
+      <c r="B13" t="s">
         <v>336</v>
-      </c>
-      <c r="B13" t="s">
-        <v>337</v>
       </c>
       <c r="C13" s="146">
         <v>1</v>
       </c>
       <c r="E13" t="s">
+        <v>337</v>
+      </c>
+      <c r="F13" t="s">
         <v>338</v>
-      </c>
-      <c r="F13" t="s">
-        <v>339</v>
       </c>
       <c r="G13" s="147">
         <v>2</v>
@@ -6199,19 +6199,19 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B14" t="s">
         <v>340</v>
-      </c>
-      <c r="B14" t="s">
-        <v>341</v>
       </c>
       <c r="C14" s="146">
         <v>1</v>
       </c>
       <c r="E14" t="s">
+        <v>341</v>
+      </c>
+      <c r="F14" t="s">
         <v>342</v>
-      </c>
-      <c r="F14" t="s">
-        <v>343</v>
       </c>
       <c r="G14" s="147">
         <v>2</v>
@@ -6219,19 +6219,19 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
+        <v>343</v>
+      </c>
+      <c r="B15" t="s">
         <v>344</v>
-      </c>
-      <c r="B15" t="s">
-        <v>345</v>
       </c>
       <c r="C15" s="146">
         <v>1</v>
       </c>
       <c r="E15" t="s">
+        <v>345</v>
+      </c>
+      <c r="F15" t="s">
         <v>346</v>
-      </c>
-      <c r="F15" t="s">
-        <v>347</v>
       </c>
       <c r="G15" s="147">
         <v>2</v>
@@ -6239,19 +6239,19 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
+        <v>347</v>
+      </c>
+      <c r="B16" t="s">
         <v>348</v>
-      </c>
-      <c r="B16" t="s">
-        <v>349</v>
       </c>
       <c r="C16" s="146">
         <v>1</v>
       </c>
       <c r="E16" t="s">
+        <v>349</v>
+      </c>
+      <c r="F16" t="s">
         <v>350</v>
-      </c>
-      <c r="F16" t="s">
-        <v>351</v>
       </c>
       <c r="G16" s="147">
         <v>2</v>
@@ -6259,19 +6259,19 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B17" t="s">
         <v>352</v>
-      </c>
-      <c r="B17" t="s">
-        <v>353</v>
       </c>
       <c r="C17" s="146">
         <v>1</v>
       </c>
       <c r="E17" t="s">
+        <v>353</v>
+      </c>
+      <c r="F17" t="s">
         <v>354</v>
-      </c>
-      <c r="F17" t="s">
-        <v>355</v>
       </c>
       <c r="G17" s="147">
         <v>2</v>
@@ -6279,7 +6279,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B18" t="s">
         <v>124</v>
@@ -6288,10 +6288,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
+        <v>356</v>
+      </c>
+      <c r="F18" t="s">
         <v>357</v>
-      </c>
-      <c r="F18" t="s">
-        <v>358</v>
       </c>
       <c r="G18" s="147">
         <v>2</v>
@@ -6299,19 +6299,19 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C19" s="146">
         <v>1</v>
       </c>
       <c r="E19" t="s">
+        <v>359</v>
+      </c>
+      <c r="F19" t="s">
         <v>360</v>
-      </c>
-      <c r="F19" t="s">
-        <v>361</v>
       </c>
       <c r="G19" s="147">
         <v>2</v>
@@ -6319,19 +6319,19 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C20" s="146">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G20" s="147">
         <v>2</v>
@@ -6339,19 +6339,19 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C21" s="146">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G21" s="147">
         <v>2</v>
@@ -6359,19 +6359,19 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>365</v>
+      </c>
+      <c r="B22" t="s">
         <v>366</v>
-      </c>
-      <c r="B22" t="s">
-        <v>367</v>
       </c>
       <c r="C22" s="146">
         <v>1</v>
       </c>
       <c r="E22" t="s">
+        <v>367</v>
+      </c>
+      <c r="F22" t="s">
         <v>368</v>
-      </c>
-      <c r="F22" t="s">
-        <v>369</v>
       </c>
       <c r="G22" s="147">
         <v>2</v>
@@ -6379,10 +6379,10 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
+        <v>369</v>
+      </c>
+      <c r="B23" t="s">
         <v>370</v>
-      </c>
-      <c r="B23" t="s">
-        <v>371</v>
       </c>
       <c r="C23" s="146">
         <v>1</v>
@@ -6390,10 +6390,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>371</v>
+      </c>
+      <c r="B24" t="s">
         <v>372</v>
-      </c>
-      <c r="B24" t="s">
-        <v>373</v>
       </c>
       <c r="C24" s="146">
         <v>1</v>
@@ -6401,10 +6401,10 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
+        <v>373</v>
+      </c>
+      <c r="B25" t="s">
         <v>374</v>
-      </c>
-      <c r="B25" t="s">
-        <v>375</v>
       </c>
       <c r="C25" s="146">
         <v>1</v>
@@ -6412,10 +6412,10 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
+        <v>375</v>
+      </c>
+      <c r="B26" t="s">
         <v>376</v>
-      </c>
-      <c r="B26" t="s">
-        <v>377</v>
       </c>
       <c r="C26" s="146">
         <v>1</v>
@@ -6423,10 +6423,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
+        <v>377</v>
+      </c>
+      <c r="B27" t="s">
         <v>378</v>
-      </c>
-      <c r="B27" t="s">
-        <v>379</v>
       </c>
       <c r="C27" s="146">
         <v>1</v>
@@ -7596,7 +7596,7 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -7621,7 +7621,7 @@
         <v>208</v>
       </c>
       <c r="H3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:8">

</xml_diff>

<commit_message>
lock cells for fiche agent
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC36EAE9-03C1-1F4B-852D-721DEC5EDD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A19CE3E-49CE-EE49-BC2D-EC58F178515C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
@@ -1297,6 +1297,10 @@
     <xf numFmtId="4" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1365,10 +1369,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1393,13 +1393,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0"/>
       </font>
@@ -1416,6 +1409,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3275,7 +3275,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="110" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3350,12 +3350,12 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="121"/>
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="133"/>
+      <c r="C6" s="133"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="134"/>
       <c r="F6" s="45" t="s">
         <v>94</v>
       </c>
@@ -3381,8 +3381,8 @@
       <c r="B8" s="122" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="134"/>
-      <c r="D8" s="135"/>
+      <c r="C8" s="135"/>
+      <c r="D8" s="136"/>
       <c r="E8" s="129" t="s">
         <v>90</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>96</v>
       </c>
       <c r="D9" s="131"/>
-      <c r="E9" s="154"/>
+      <c r="E9" s="132"/>
       <c r="F9" t="s">
         <v>99</v>
       </c>
@@ -3417,25 +3417,25 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="AyMUXgNitMi7oeKL4dEzZMxeOT0h77bozqCg1qZa01QpuIA7aVRhZeQPkev1wTb7QocDVW49HvjevabbKaTUUQ==" saltValue="sc2K/AYp/26JQKUdfyEyyQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="2">
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C8:D8"/>
   </mergeCells>
+  <conditionalFormatting sqref="A9:E200">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+      <formula>$A9=""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B7:E7">
-    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="14" stopIfTrue="1">
       <formula>$E$7&lt;&gt;100%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:E200">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$C9=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:E200">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>$A9=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C200">
@@ -3547,10 +3547,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="27"/>
-      <c r="F4" s="141" t="s">
+      <c r="F4" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="142"/>
+      <c r="G4" s="143"/>
       <c r="H4" s="71"/>
       <c r="I4" s="2">
         <v>208</v>
@@ -3561,10 +3561,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1">
-      <c r="F5" s="143" t="s">
+      <c r="F5" s="144" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="144"/>
+      <c r="G5" s="145"/>
       <c r="H5" s="72"/>
       <c r="I5" s="6">
         <v>8</v>
@@ -3580,28 +3580,28 @@
       <c r="H6" s="35"/>
     </row>
     <row r="7" spans="2:12" ht="70" customHeight="1">
-      <c r="B7" s="139" t="s">
+      <c r="B7" s="140" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="138" t="s">
+      <c r="E7" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="138"/>
+      <c r="F7" s="139"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="136" t="s">
+      <c r="I7" s="137" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="69"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1">
-      <c r="B8" s="140"/>
-      <c r="I8" s="137"/>
+      <c r="B8" s="141"/>
+      <c r="I8" s="138"/>
       <c r="J8" s="70"/>
       <c r="L8"/>
     </row>
@@ -3643,7 +3643,7 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="2:12" ht="69" customHeight="1">
-      <c r="B12" s="139" t="s">
+      <c r="B12" s="140" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="32" t="s">
@@ -3659,11 +3659,11 @@
       <c r="L12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B13" s="140"/>
+      <c r="B13" s="141"/>
       <c r="C13" s="77"/>
       <c r="D13" s="77"/>
       <c r="E13" s="73"/>
-      <c r="G13" s="137" t="s">
+      <c r="G13" s="138" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="70"/>
@@ -3678,7 +3678,7 @@
       <c r="E14" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="137"/>
+      <c r="G14" s="138"/>
       <c r="H14" s="70"/>
       <c r="I14" s="10"/>
     </row>
@@ -3808,14 +3808,14 @@
       </c>
       <c r="C3" s="114"/>
       <c r="D3" s="26"/>
-      <c r="F3" s="145" t="s">
+      <c r="F3" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="148"/>
       <c r="L3"/>
     </row>
     <row r="4" spans="2:12" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
@@ -3824,10 +3824,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="27"/>
-      <c r="F4" s="141" t="s">
+      <c r="F4" s="142" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="142"/>
+      <c r="G4" s="143"/>
       <c r="H4" s="71"/>
       <c r="I4" s="10">
         <v>1607</v>
@@ -3838,10 +3838,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="F5" s="143" t="s">
+      <c r="F5" s="144" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="144"/>
+      <c r="G5" s="145"/>
       <c r="H5" s="72"/>
       <c r="I5" s="104">
         <v>35</v>
@@ -3858,28 +3858,28 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="70" customHeight="1">
-      <c r="B7" s="139" t="s">
+      <c r="B7" s="140" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="138" t="s">
+      <c r="E7" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="138"/>
+      <c r="F7" s="139"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="136" t="s">
+      <c r="I7" s="137" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="69"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1">
-      <c r="B8" s="140"/>
-      <c r="I8" s="137"/>
+      <c r="B8" s="141"/>
+      <c r="I8" s="138"/>
       <c r="J8" s="70"/>
       <c r="L8"/>
     </row>
@@ -3922,7 +3922,7 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="2:12" ht="69" customHeight="1">
-      <c r="B12" s="139" t="s">
+      <c r="B12" s="140" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="118" t="s">
@@ -3938,11 +3938,11 @@
       <c r="L12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B13" s="140"/>
+      <c r="B13" s="141"/>
       <c r="C13" s="119"/>
       <c r="D13" s="77"/>
       <c r="E13" s="73"/>
-      <c r="G13" s="137" t="s">
+      <c r="G13" s="138" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="70"/>
@@ -3957,7 +3957,7 @@
       <c r="E14" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="137"/>
+      <c r="G14" s="138"/>
       <c r="H14" s="70"/>
       <c r="I14" s="10"/>
     </row>
@@ -4072,30 +4072,30 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="3:9" ht="54.75" customHeight="1">
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="150" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
     </row>
     <row r="3" spans="3:9" ht="27.75" customHeight="1">
       <c r="C3" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="148" t="s">
+      <c r="D3" s="149" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="148"/>
-      <c r="F3" s="150" t="s">
+      <c r="E3" s="149"/>
+      <c r="F3" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
     </row>
     <row r="4" spans="3:9" ht="23.25" customHeight="1">
       <c r="C4" s="40" t="s">
@@ -4350,26 +4350,26 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="3:12" ht="46.5" customHeight="1">
-      <c r="E2" s="151" t="s">
+      <c r="E2" s="152" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
     </row>
     <row r="3" spans="3:12" ht="53.25" customHeight="1">
-      <c r="E3" s="152" t="s">
+      <c r="E3" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
-      <c r="K3" s="152"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
     </row>
     <row r="4" spans="3:12" ht="20.75" customHeight="1">
       <c r="E4" s="61"/>
@@ -4428,10 +4428,10 @@
       <c r="I8" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="150" t="s">
+      <c r="J8" s="151" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="150"/>
+      <c r="K8" s="151"/>
     </row>
     <row r="9" spans="3:12" ht="14" customHeight="1">
       <c r="D9" s="39"/>
@@ -4451,11 +4451,11 @@
       <c r="H10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="153" t="s">
+      <c r="I10" s="154" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="153"/>
-      <c r="K10" s="153"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="154"/>
     </row>
     <row r="11" spans="3:12" customFormat="1" ht="14.75" customHeight="1">
       <c r="E11" s="50"/>

</xml_diff>

<commit_message>
protect file fiche agent
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -8,7 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A19CE3E-49CE-EE49-BC2D-EC58F178515C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA21F0CE-A96B-5F46-B6AB-35149B057A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="AeHGh/AdW5GzWqeec99QpeLsXaxf0i6xyyOFGoQ2PSeXpiAEKbfBAJpWmi8zD9Zb2nHd0xthIuor8DCAYfnN3g==" workbookSaltValue="nUTU23Jr2g9V5YK7BWZMZA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
@@ -3730,7 +3731,7 @@
       <c r="D19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="qoKeuRyEHA2nvkK6SFR92jOmDvBgvBN0dULItng4BOKYj2SreqFORsdD+7KksFG5eLiTERecYW0N2rBhhAC/Kw==" saltValue="FWgK0l1kHyAeMX8O1xW5+A==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="E7:F7"/>
@@ -4009,7 +4010,7 @@
       <c r="D19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Fmw8SxcEHmkmuKfZIDlG3lUf38K+B0ycq7UXLx0ydjFDAFQK16CMXX3SWzc6v1FFvFi902Pbnd/D9gaP8dv7EA==" saltValue="idF5T1PQ/ZQDUyep3u1FXA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="8">
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="I7:I8"/>
@@ -4295,7 +4296,7 @@
       <c r="C22" s="48"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oCjaO8guuJZW51bOq0YeyMWFkAyRqslg/2h+jl80NCowOGxnzokuhQ5KrhMRASTQCjl1FiL5zuJTOmlN6Zvoyg==" saltValue="xw0UIWyYJFPuZalQhkxaYQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="C2:I2"/>
@@ -4590,7 +4591,7 @@
       <c r="L19" s="100"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="e13rMI8cCcOwpXK2/xjTVPCn91cEskZ8kyQ4IkPQTjm5/WntfCwbZauJQJKfGC4tCTTGzv83yDff/tB+07iSIQ==" saltValue="/KhouqfTR1M83iTX114muQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="E2:K2"/>

</xml_diff>

<commit_message>
update label fiche agent autour du magistrat
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA21F0CE-A96B-5F46-B6AB-35149B057A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312B8D54-E2DD-7F4F-BEE2-26E1FD9E0DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="AeHGh/AdW5GzWqeec99QpeLsXaxf0i6xyyOFGoQ2PSeXpiAEKbfBAJpWmi8zD9Zb2nHd0xthIuor8DCAYfnN3g==" workbookSaltValue="nUTU23Jr2g9V5YK7BWZMZA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
@@ -3418,7 +3418,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="AyMUXgNitMi7oeKL4dEzZMxeOT0h77bozqCg1qZa01QpuIA7aVRhZeQPkev1wTb7QocDVW49HvjevabbKaTUUQ==" saltValue="sc2K/AYp/26JQKUdfyEyyQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+eBRqPR7CCk4zHyrlyag+yZqOt/qouVJ231b5OXN6NA9wb+eDnsahcW3kYyzxck8GGAFYYVjcwZbti6bnJ3iqw==" saltValue="0LwqBRJn4gGMC7PfXtNYTw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="2">
     <mergeCell ref="B6:E6"/>
@@ -3451,7 +3451,7 @@
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Erreur de saisie" error="Vous devez choisir une fonction dans la liste proposée !" sqref="C4" xr:uid="{4B86F8E2-A2C1-4AF0-8AD2-6F6FB121C7E1}">
-      <formula1>INDIRECT(SUBSTITUTE($C$2,"N"," "))</formula1>
+      <formula1>INDIRECT(SUBSTITUTE($C$2," ","_"))</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date non valide" error="Saisir une date au format JJ/MM/AAAA" sqref="C8" xr:uid="{A91592D5-FAF1-48BE-B5FE-60B612F0C2AB}">
       <formula1>1</formula1>

</xml_diff>

<commit_message>
update Feuille de temps Modèle %
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312B8D54-E2DD-7F4F-BEE2-26E1FD9E0DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="AeHGh/AdW5GzWqeec99QpeLsXaxf0i6xyyOFGoQ2PSeXpiAEKbfBAJpWmi8zD9Zb2nHd0xthIuor8DCAYfnN3g==" workbookSaltValue="nUTU23Jr2g9V5YK7BWZMZA==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980DD5D6-D2DB-B14A-A97D-7083FC7AC889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille de temps" sheetId="8" r:id="rId1"/>
     <sheet name="Fonction" sheetId="10" state="hidden" r:id="rId2"/>
-    <sheet name="Magistrats" sheetId="3" r:id="rId3"/>
-    <sheet name="Fonctionnaires" sheetId="4" r:id="rId4"/>
+    <sheet name="Calculatrice magistrats" sheetId="3" r:id="rId3"/>
+    <sheet name="Calculatrice fonctionnaires" sheetId="4" r:id="rId4"/>
     <sheet name="Reconvertir % d'ETPT" sheetId="5" r:id="rId5"/>
-    <sheet name="Convertir ETPT en audiences" sheetId="7" r:id="rId6"/>
-    <sheet name="Listes" sheetId="2" state="hidden" r:id="rId7"/>
+    <sheet name="Listes" sheetId="2" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="AUTOUR_DU_MAGISTRAT">Fonction!$C$1:$C$100</definedName>
@@ -47,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="86">
   <si>
     <t>Temps de travail d'un magistrat</t>
   </si>
@@ -313,199 +311,6 @@
     <t>* étant considéré comme un mois : un douzième d'année, soit un mois moyen, congés payés déduits</t>
   </si>
   <si>
-    <t>ETPT</t>
-  </si>
-  <si>
-    <t>qui tenaient</t>
-  </si>
-  <si>
-    <t>(sélectionner la fréquence dans le menu déroulant qui apparaît en cliquant sur la case jaune)</t>
-  </si>
-  <si>
-    <t>ETPT*</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Jusqu'ici</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, pour ce contentieux,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je mobilisais</t>
-    </r>
-  </si>
-  <si>
-    <t>à ce contentieux</t>
-  </si>
-  <si>
-    <t>* ETPT dont l'activité, et particulièrement le temps consacré aux audiences, serait similaire à ceux affectés précédemment.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ce qui </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>devrait permettre,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> proportionnellement, de tenir</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">soit un </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>total</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> de</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cette méthode est bien entendu très approximative et ne tient par exemple pas compte de la complexité de la création d'audiences supplémentaires (disponibilité des salles, des effectifs de greffe ou de magistrats habilités à présider des audiences...). Elle ne fait qu'appliquer une règle de proportionnalité : </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Si, jusqu'à maintenant, xx ETPT affectés à un contentieux permettaient de tenir X audiences, alors, l'affectation de yy ETPT devrait permettre d'envisager la tenue de Y audiences.</t>
-    </r>
-  </si>
-  <si>
-    <t>Si vous envisagez d'affecter des effectifs supplémentaires à un contentieux ou, au contraire, devez limiter les ETPT s'y consacrant, 
-nous vous proposons 1 méthode simple  pour estimer le nombre d'audiences qui pourraient être tenues par la nouvelle équipe.</t>
-  </si>
-  <si>
-    <r>
-      <t>Dans cette simulation, j'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">envisage </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">d'affecter à ce </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>contentieux</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">renseigner les cases jaunes </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dans ma simulation, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>je prévois donc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> d'affecter </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> au total</t>
-  </si>
-  <si>
     <t>Catégorie</t>
   </si>
   <si>
@@ -578,6 +383,9 @@
   <si>
     <t>#! END_LOOP c</t>
   </si>
+  <si>
+    <t>%</t>
+  </si>
 </sst>
 </file>
 
@@ -591,7 +399,7 @@
     <numFmt numFmtId="168" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,30 +453,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -918,7 +702,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -983,7 +767,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1003,10 +786,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1056,54 +835,8 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1126,7 +859,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1180,71 +913,13 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1263,56 +938,56 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="13" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="13" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="14" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="18" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="15" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1362,14 +1037,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2804,167 +2483,6 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="1905000" cy="1847850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>60007</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>51403</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>655309</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB5DD342-154A-47AE-B83E-9A4DE4C8C1E4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="60007" y="0"/>
-          <a:ext cx="1538256" cy="1478280"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>100007</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>214072</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>601966</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>5702</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Graphique 1" descr="Jouer avec un remplissage uni">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A6D8287-765F-4C02-B462-1CF623E55EBD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="6419727" y="1628652"/>
-          <a:ext cx="326944" cy="500063"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>3802374</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>15241</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>66638</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>482399</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Graphique 3" descr="Jouer avec un remplissage uni">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E565DA-270E-4BE0-B6F7-696063E5D3B7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="6600109" y="3145866"/>
-          <a:ext cx="463356" cy="922945"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3290,131 +2808,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" hidden="1">
-      <c r="A1" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="121"/>
+      <c r="A1" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="86"/>
       <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="33" customHeight="1">
-      <c r="A2" s="121"/>
-      <c r="B2" s="122" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="124"/>
-      <c r="F2" s="42"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="88"/>
+      <c r="D2" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="89"/>
+      <c r="F2" s="40"/>
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1">
-      <c r="A3" s="121"/>
-      <c r="B3" s="122" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="123"/>
-      <c r="D3" s="45" t="s">
-        <v>94</v>
+      <c r="A3" s="86"/>
+      <c r="B3" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="88"/>
+      <c r="D3" s="43" t="s">
+        <v>79</v>
       </c>
       <c r="E3" s="13"/>
-      <c r="F3" s="42"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:7" ht="33" customHeight="1">
-      <c r="A4" s="121"/>
-      <c r="B4" s="122" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="123"/>
-      <c r="D4" s="45" t="s">
-        <v>94</v>
+      <c r="A4" s="86"/>
+      <c r="B4" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="88"/>
+      <c r="D4" s="43" t="s">
+        <v>79</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="42"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="13"/>
     </row>
     <row r="5" spans="1:7" ht="31" customHeight="1" thickBot="1">
-      <c r="A5" s="121"/>
-      <c r="B5" s="122" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="122" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="125"/>
-      <c r="F5" s="45" t="s">
-        <v>94</v>
+      <c r="A5" s="86"/>
+      <c r="B5" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="88"/>
+      <c r="D5" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="90"/>
+      <c r="F5" s="43" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="121"/>
-      <c r="B6" s="133" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="133"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="45" t="s">
-        <v>94</v>
+      <c r="A6" s="86"/>
+      <c r="B6" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="43" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="110" customHeight="1" thickTop="1">
       <c r="A7" s="10"/>
-      <c r="B7" s="126" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="126" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="127" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="128"/>
-      <c r="F7" s="45" t="s">
-        <v>94</v>
+      <c r="B7" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="92" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="93"/>
+      <c r="F7" s="43" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="42" customHeight="1">
       <c r="A8" s="10"/>
-      <c r="B8" s="122" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="135"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="129" t="s">
-        <v>90</v>
+      <c r="B8" s="87" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="100"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="94" t="s">
+        <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="130" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="131" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="131"/>
-      <c r="E9" s="132"/>
+        <v>83</v>
+      </c>
+      <c r="B9" s="95" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="96" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="96"/>
+      <c r="E9" s="97"/>
       <c r="F9" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="F10" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="F11" s="13" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3496,7 +3014,7 @@
   <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3504,7 +3022,7 @@
     <col min="1" max="1" width="33.33203125" customWidth="1"/>
     <col min="2" max="2" width="53.33203125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="1.33203125" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
@@ -3523,17 +3041,19 @@
       <c r="F2" s="19"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="78"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="4"/>
       <c r="K2" s="5"/>
       <c r="L2"/>
     </row>
     <row r="3" spans="2:12" ht="40.5" customHeight="1">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="26"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="117" t="s">
+        <v>85</v>
+      </c>
       <c r="F3" s="18" t="s">
         <v>19</v>
       </c>
@@ -3543,16 +3063,16 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="2:12" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B4" s="29"/>
-      <c r="C4" s="30" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="F4" s="142" t="s">
+      <c r="D4" s="26"/>
+      <c r="F4" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="143"/>
-      <c r="H4" s="71"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="2">
         <v>208</v>
       </c>
@@ -3562,69 +3082,69 @@
       </c>
     </row>
     <row r="5" spans="2:12" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1">
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="145"/>
-      <c r="H5" s="72"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="55"/>
       <c r="I5" s="6">
         <v>8</v>
       </c>
-      <c r="J5" s="37"/>
+      <c r="J5" s="35"/>
       <c r="K5" s="12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="20.75" customHeight="1" thickBot="1">
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="2:12" ht="70" customHeight="1">
-      <c r="B7" s="140" t="s">
+      <c r="B7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="139" t="s">
+      <c r="E7" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="139"/>
+      <c r="F7" s="104"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="137" t="s">
+      <c r="I7" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="69"/>
+      <c r="J7" s="52"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1">
-      <c r="B8" s="141"/>
-      <c r="I8" s="138"/>
-      <c r="J8" s="70"/>
+      <c r="B8" s="106"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="53"/>
       <c r="L8"/>
     </row>
     <row r="9" spans="2:12" ht="38.25" customHeight="1">
       <c r="B9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="115"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="75" t="s">
+      <c r="E9" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="75" t="s">
+      <c r="F9" s="58" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="80" t="str">
+      <c r="I9" s="63" t="str">
         <f>IF($C$3="","",(C9*(VLOOKUP(E9,Listes!$A$2:$B$5,2,FALSE))*VLOOKUP(F9,Listes!$C$2:$D$6,2,FALSE))/($I$4*$C$3))</f>
         <v/>
       </c>
-      <c r="J9" s="76"/>
+      <c r="J9" s="59"/>
       <c r="L9"/>
     </row>
     <row r="10" spans="2:12" ht="9.75" customHeight="1" thickBot="1">
@@ -3635,7 +3155,7 @@
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
-      <c r="I10" s="74"/>
+      <c r="I10" s="57"/>
       <c r="J10" s="25"/>
       <c r="L10"/>
     </row>
@@ -3644,51 +3164,51 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="2:12" ht="69" customHeight="1">
-      <c r="B12" s="140" t="s">
+      <c r="B12" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="31" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="17"/>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="31" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="78"/>
+      <c r="G12" s="61"/>
       <c r="H12" s="5"/>
       <c r="L12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B13" s="141"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="73"/>
-      <c r="G13" s="138" t="s">
+      <c r="B13" s="106"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="56"/>
+      <c r="G13" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="70"/>
+      <c r="H13" s="53"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="2:12" s="3" customFormat="1" ht="40.25" customHeight="1">
       <c r="B14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="115"/>
+      <c r="C14" s="80"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="75" t="s">
+      <c r="E14" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="138"/>
-      <c r="H14" s="70"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="53"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="2:12" s="3" customFormat="1" ht="6.75" customHeight="1">
       <c r="B15" s="15"/>
-      <c r="C15" s="120"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="G15" s="77"/>
+      <c r="G15" s="60"/>
       <c r="H15" s="9"/>
       <c r="I15" s="10"/>
     </row>
@@ -3696,12 +3216,12 @@
       <c r="B16" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="115"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="75" t="s">
+      <c r="E16" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="80" t="str">
+      <c r="G16" s="63" t="str">
         <f>IF($C$3="","",(C14*VLOOKUP(E14,Listes!A2:B5,2,FALSE))*C16*VLOOKUP(E16,Listes!C2:D6,2,FALSE)/($I$4*$C$3))</f>
         <v/>
       </c>
@@ -3714,12 +3234,12 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="79"/>
+      <c r="G17" s="62"/>
       <c r="H17" s="8"/>
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="2:9" ht="18" customHeight="1">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="13"/>
@@ -3731,7 +3251,7 @@
       <c r="D19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qoKeuRyEHA2nvkK6SFR92jOmDvBgvBN0dULItng4BOKYj2SreqFORsdD+7KksFG5eLiTERecYW0N2rBhhAC/Kw==" saltValue="FWgK0l1kHyAeMX8O1xW5+A==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jqBc884VA69ze/2tSZDU+ADryz+4MAF600EV711jEgXI7Nv4bB92an8i2JXOYp+XDJduwYELbs4ANtFz0O7InQ==" saltValue="Sm6fC5DKcUI9p4Z0MWslWw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="E7:F7"/>
@@ -3779,7 +3299,7 @@
     <col min="1" max="1" width="33.33203125" customWidth="1"/>
     <col min="2" max="2" width="53.33203125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="1.33203125" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
@@ -3798,107 +3318,109 @@
       <c r="F2" s="19"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="78"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="4"/>
       <c r="K2" s="5"/>
       <c r="L2"/>
     </row>
     <row r="3" spans="2:12" ht="40.5" customHeight="1">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="26"/>
-      <c r="F3" s="146" t="s">
+      <c r="C3" s="118"/>
+      <c r="D3" s="117" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147"/>
-      <c r="J3" s="147"/>
-      <c r="K3" s="148"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="113"/>
       <c r="L3"/>
     </row>
     <row r="4" spans="2:12" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B4" s="29"/>
-      <c r="C4" s="30" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="F4" s="142" t="s">
+      <c r="D4" s="26"/>
+      <c r="F4" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="143"/>
-      <c r="H4" s="71"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="10">
         <v>1607</v>
       </c>
       <c r="J4" s="1"/>
-      <c r="K4" s="90" t="s">
+      <c r="K4" s="73" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:12" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="145"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="104">
+      <c r="G5" s="110"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="119">
         <v>35</v>
       </c>
-      <c r="J5" s="34"/>
-      <c r="K5" s="105" t="s">
+      <c r="J5" s="120"/>
+      <c r="K5" s="77" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30.5" customHeight="1" thickBot="1">
-      <c r="F6" s="35"/>
-      <c r="K6" s="36" t="s">
+      <c r="F6" s="33"/>
+      <c r="K6" s="34" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="70" customHeight="1">
-      <c r="B7" s="140" t="s">
+      <c r="B7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="139" t="s">
+      <c r="E7" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="139"/>
+      <c r="F7" s="104"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="137" t="s">
+      <c r="I7" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="69"/>
+      <c r="J7" s="52"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1">
-      <c r="B8" s="141"/>
-      <c r="I8" s="138"/>
-      <c r="J8" s="70"/>
+      <c r="B8" s="106"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="53"/>
       <c r="L8"/>
     </row>
     <row r="9" spans="2:12" ht="38.25" customHeight="1">
       <c r="B9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="115"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="75" t="s">
+      <c r="E9" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="75" t="s">
+      <c r="F9" s="58" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="80" t="str">
+      <c r="I9" s="63" t="str">
         <f>IF($C$3="","",(C9*(VLOOKUP(E9,Listes!$A$9:$B$12,2,FALSE))*VLOOKUP(F9,Listes!$C$9:$D$13,2,FALSE))/(($I$4)*$C$3))</f>
         <v/>
       </c>
@@ -3907,67 +3429,67 @@
     </row>
     <row r="10" spans="2:12" ht="9.75" customHeight="1" thickBot="1">
       <c r="B10" s="23"/>
-      <c r="C10" s="116"/>
+      <c r="C10" s="81"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
-      <c r="I10" s="74"/>
+      <c r="I10" s="57"/>
       <c r="J10" s="25"/>
       <c r="L10"/>
     </row>
     <row r="11" spans="2:12" ht="7.25" customHeight="1" thickBot="1">
-      <c r="C11" s="117"/>
+      <c r="C11" s="82"/>
       <c r="J11" s="2"/>
       <c r="L11"/>
     </row>
     <row r="12" spans="2:12" ht="69" customHeight="1">
-      <c r="B12" s="140" t="s">
+      <c r="B12" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="118" t="s">
+      <c r="C12" s="83" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="17"/>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="31" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="78"/>
+      <c r="G12" s="61"/>
       <c r="H12" s="5"/>
       <c r="L12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B13" s="141"/>
-      <c r="C13" s="119"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="73"/>
-      <c r="G13" s="138" t="s">
+      <c r="B13" s="106"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="56"/>
+      <c r="G13" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="70"/>
+      <c r="H13" s="53"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="2:12" s="3" customFormat="1" ht="33" customHeight="1">
       <c r="B14" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="115"/>
+      <c r="C14" s="80"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="75" t="s">
+      <c r="E14" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="138"/>
-      <c r="H14" s="70"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="53"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="2:12" s="3" customFormat="1" ht="12" customHeight="1">
       <c r="B15" s="15"/>
-      <c r="C15" s="120"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="G15" s="81"/>
+      <c r="G15" s="64"/>
       <c r="H15" s="9"/>
       <c r="I15" s="10"/>
     </row>
@@ -3975,12 +3497,12 @@
       <c r="B16" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="115"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="75" t="s">
+      <c r="E16" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="82" t="str">
+      <c r="G16" s="65" t="str">
         <f>IF($C$3="","",(C14*VLOOKUP(E14,Listes!A9:B12,2,FALSE))*C16*VLOOKUP(E16,Listes!C9:D13,2,FALSE)/($I$4*$C$3))</f>
         <v/>
       </c>
@@ -3993,12 +3515,12 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="79"/>
+      <c r="G17" s="62"/>
       <c r="H17" s="8"/>
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="2:9" ht="18" customHeight="1">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="13"/>
@@ -4010,7 +3532,7 @@
       <c r="D19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Fmw8SxcEHmkmuKfZIDlG3lUf38K+B0ycq7UXLx0ydjFDAFQK16CMXX3SWzc6v1FFvFi902Pbnd/D9gaP8dv7EA==" saltValue="idF5T1PQ/ZQDUyep3u1FXA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="KvRyNI6PwNUPf4sBKQmwTWJsBl6DRSAtCfG8PI0Ffbx/o6tCdZdNraKNIaedl71P9bQ9zlSKQZDVBY5tfz8qBQ==" saltValue="Ypq0yF5Zv9isQZHgL9Uktg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="8">
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="I7:I8"/>
@@ -4057,10 +3579,10 @@
   <cols>
     <col min="1" max="1" width="12" style="3" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="43.5" style="50" customWidth="1"/>
+    <col min="3" max="3" width="43.5" style="48" customWidth="1"/>
     <col min="4" max="4" width="9" style="3" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="43" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="41" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" style="3"/>
     <col min="9" max="9" width="22.33203125" style="3" customWidth="1"/>
@@ -4073,227 +3595,227 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="3:9" ht="54.75" customHeight="1">
-      <c r="C2" s="150" t="s">
+      <c r="C2" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
     </row>
     <row r="3" spans="3:9" ht="27.75" customHeight="1">
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="149" t="s">
+      <c r="D3" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="149"/>
-      <c r="F3" s="151" t="s">
+      <c r="E3" s="114"/>
+      <c r="F3" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
-      <c r="I3" s="151"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
     </row>
     <row r="4" spans="3:9" ht="23.25" customHeight="1">
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="41" t="str">
+      <c r="D4" s="39" t="str">
         <f>IF(D3="FONCTIONNAIRE","1607 h/an et 35h/semaine","208 jours/an et 8 h/jour")</f>
         <v>208 jours/an et 8 h/jour</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="43"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" spans="3:9" ht="7.5" customHeight="1">
-      <c r="C5" s="39"/>
-      <c r="D5" s="41"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="3"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="43"/>
+      <c r="G5" s="41"/>
     </row>
     <row r="6" spans="3:9" ht="23.25" customHeight="1">
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="113"/>
-      <c r="E6" s="44" t="s">
+      <c r="D6" s="79"/>
+      <c r="E6" s="42" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
     </row>
     <row r="7" spans="3:9" ht="25.25" customHeight="1">
-      <c r="C7" s="39"/>
-      <c r="D7" s="83" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="44"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
     </row>
     <row r="8" spans="3:9" ht="24" customHeight="1">
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="113"/>
-      <c r="E8" s="44" t="s">
+      <c r="D8" s="79"/>
+      <c r="E8" s="42" t="s">
         <v>44</v>
       </c>
       <c r="F8" s="10"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
     </row>
     <row r="9" spans="3:9" ht="18" customHeight="1">
-      <c r="C9" s="39"/>
-      <c r="D9" s="84" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="44"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
     </row>
     <row r="10" spans="3:9" ht="36" customHeight="1" thickBot="1">
-      <c r="C10" s="39"/>
-      <c r="D10" s="47"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="45"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="3:9" ht="7.25" customHeight="1">
-      <c r="C11" s="86"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="89"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="72"/>
     </row>
     <row r="12" spans="3:9" ht="24" customHeight="1">
       <c r="C12" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="106">
-        <f>IF(D3="MAGISTRAT",D6*D8*Listes!D3,D6*D8*Fonctionnaires!I4/7)</f>
+      <c r="D12" s="78">
+        <f>IF(D3="MAGISTRAT",D6*D8*Listes!D3,D6*D8*'Calculatrice fonctionnaires'!I4/7)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="42" t="s">
         <v>47</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="106">
+      <c r="G12" s="78">
         <f>IF(D3="FONCTIONNAIRE",D12*7,D12*8)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="44" t="s">
+      <c r="H12" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="90"/>
+      <c r="I12" s="73"/>
     </row>
     <row r="13" spans="3:9" ht="8.25" customHeight="1">
       <c r="C13" s="15"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="44"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="90"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="3:9" ht="24" customHeight="1">
       <c r="C14" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="106">
+      <c r="D14" s="78">
         <f>D12/12</f>
         <v>0</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="42" t="s">
         <v>59</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="106">
+      <c r="G14" s="78">
         <f>IF(D4="FONCTIONNAIRE",D14*7,D14*8)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="44" t="s">
+      <c r="H14" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="90"/>
+      <c r="I14" s="73"/>
     </row>
     <row r="15" spans="3:9" ht="6.75" customHeight="1">
       <c r="C15" s="15"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="44"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="90"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="73"/>
     </row>
     <row r="16" spans="3:9" ht="24" customHeight="1">
       <c r="C16" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="106">
+      <c r="D16" s="78">
         <f>(D8*D6)*5</f>
         <v>0</v>
       </c>
-      <c r="E16" s="44" t="s">
+      <c r="E16" s="42" t="s">
         <v>61</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="106">
+      <c r="G16" s="78">
         <f>IF(D3="FONCTIONNAIRE",D16*7,D16*8)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="44" t="s">
+      <c r="H16" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="I16" s="90"/>
+      <c r="I16" s="73"/>
     </row>
     <row r="17" spans="3:9" ht="9" customHeight="1" thickBot="1">
-      <c r="C17" s="91"/>
-      <c r="D17" s="92"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="75"/>
       <c r="E17" s="7"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="93"/>
+      <c r="G17" s="76"/>
       <c r="H17" s="7"/>
       <c r="I17" s="12"/>
     </row>
     <row r="18" spans="3:9" ht="16.25" customHeight="1">
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="49" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="3:9" ht="16.25" customHeight="1">
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="49" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="20" spans="3:9" ht="24" customHeight="1">
-      <c r="C20" s="48"/>
+      <c r="C20" s="46"/>
     </row>
     <row r="21" spans="3:9" ht="24" customHeight="1">
-      <c r="C21" s="49"/>
+      <c r="C21" s="47"/>
     </row>
     <row r="22" spans="3:9" ht="24" customHeight="1">
-      <c r="C22" s="48"/>
+      <c r="C22" s="46"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="oCjaO8guuJZW51bOq0YeyMWFkAyRqslg/2h+jl80NCowOGxnzokuhQ5KrhMRASTQCjl1FiL5zuJTOmlN6Zvoyg==" saltValue="xw0UIWyYJFPuZalQhkxaYQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
@@ -4321,302 +3843,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480D2DAB-0DEC-4435-9DCE-D139DCBCA90F}">
-  <dimension ref="C1:L19"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="24" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="11.33203125" style="3"/>
-    <col min="2" max="2" width="0.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="2" style="3" customWidth="1"/>
-    <col min="5" max="5" width="54.6640625" style="50" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="0.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" style="43" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="38.33203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="2" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.33203125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="3:12" ht="18" customHeight="1">
-      <c r="E1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="3:12" ht="46.5" customHeight="1">
-      <c r="E2" s="152" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
-    </row>
-    <row r="3" spans="3:12" ht="53.25" customHeight="1">
-      <c r="E3" s="153" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
-      <c r="J3" s="153"/>
-      <c r="K3" s="153"/>
-    </row>
-    <row r="4" spans="3:12" ht="20.75" customHeight="1">
-      <c r="E4" s="61"/>
-      <c r="F4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="61"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-    </row>
-    <row r="5" spans="3:12" ht="21.5" customHeight="1">
-      <c r="E5" s="61"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-    </row>
-    <row r="6" spans="3:12" ht="23.25" customHeight="1">
-      <c r="E6" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="107"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" s="53"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="45"/>
-    </row>
-    <row r="7" spans="3:12" ht="5.75" customHeight="1">
-      <c r="E7" s="39"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="45"/>
-    </row>
-    <row r="8" spans="3:12" ht="26" customHeight="1">
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="107"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="10" t="str">
-        <f>IF(F8&lt;2,"audience","audiences")</f>
-        <v>audience</v>
-      </c>
-      <c r="I8" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="151" t="s">
-        <v>67</v>
-      </c>
-      <c r="K8" s="151"/>
-    </row>
-    <row r="9" spans="3:12" ht="14" customHeight="1">
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="109"/>
-      <c r="G9" s="62"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="45"/>
-    </row>
-    <row r="10" spans="3:12" ht="23.25" customHeight="1">
-      <c r="E10" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="107"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="154" t="s">
-        <v>79</v>
-      </c>
-      <c r="J10" s="154"/>
-      <c r="K10" s="154"/>
-    </row>
-    <row r="11" spans="3:12" customFormat="1" ht="14.75" customHeight="1">
-      <c r="E11" s="50"/>
-      <c r="F11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="103"/>
-    </row>
-    <row r="12" spans="3:12" ht="39.75" customHeight="1" thickBot="1">
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="3:12" ht="5.75" customHeight="1">
-      <c r="D13" s="94"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="96"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="100"/>
-    </row>
-    <row r="14" spans="3:12" ht="24" customHeight="1">
-      <c r="C14" s="64"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="110" t="str">
-        <f>IF(F10="","",ABS(F10-F6))</f>
-        <v/>
-      </c>
-      <c r="G14" s="58"/>
-      <c r="H14" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="101" t="str">
-        <f>IF(F14="","",IF((F10-F6)&gt;=2,"supplémentaires",IF((F10-F6)&gt;0,"supplémentaire","en moins")))</f>
-        <v/>
-      </c>
-      <c r="J14" s="102" t="s">
-        <v>70</v>
-      </c>
-      <c r="K14" s="90"/>
-      <c r="L14" s="100"/>
-    </row>
-    <row r="15" spans="3:12" ht="6" customHeight="1">
-      <c r="C15" s="64"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="58"/>
-      <c r="I15" s="101"/>
-      <c r="J15" s="102"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="100"/>
-    </row>
-    <row r="16" spans="3:12" ht="24" customHeight="1">
-      <c r="C16" s="64"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="110" t="str">
-        <f>IF(F14="","",ABS(F8*F14/F6))</f>
-        <v/>
-      </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="10" t="str">
-        <f>IF(F16&lt;2,"audience","audiences")</f>
-        <v>audiences</v>
-      </c>
-      <c r="I16" s="101" t="str">
-        <f>IF(F16="","",IF((F10-F6)&lt;0,"en moins",IF(F16&gt;=2,"supplémentaires","supplémentaire")))</f>
-        <v/>
-      </c>
-      <c r="J16" s="102" t="str">
-        <f>IF(I16="","",I8)</f>
-        <v/>
-      </c>
-      <c r="K16" s="90" t="str">
-        <f>IF(J16="","","(toutes choses restant égales par ailleurs)")</f>
-        <v/>
-      </c>
-      <c r="L16" s="100"/>
-    </row>
-    <row r="17" spans="3:12" ht="5.25" customHeight="1">
-      <c r="C17" s="64"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="59"/>
-      <c r="I17" s="101"/>
-      <c r="J17" s="102"/>
-      <c r="K17" s="90"/>
-      <c r="L17" s="100"/>
-    </row>
-    <row r="18" spans="3:12" ht="24" customHeight="1">
-      <c r="C18" s="64"/>
-      <c r="D18" s="97"/>
-      <c r="E18" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="110" t="str">
-        <f>IF(OR(F10=0,F6=0),"",F8/F6*F10)</f>
-        <v/>
-      </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="10" t="str">
-        <f>IF(F18&lt;2,"audience","audiences")</f>
-        <v>audiences</v>
-      </c>
-      <c r="I18" s="101" t="str">
-        <f>J16</f>
-        <v/>
-      </c>
-      <c r="J18" s="102"/>
-      <c r="K18" s="90"/>
-      <c r="L18" s="100"/>
-    </row>
-    <row r="19" spans="3:12" ht="6.5" customHeight="1" thickBot="1">
-      <c r="C19" s="66"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="99"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="100"/>
-    </row>
-  </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="e13rMI8cCcOwpXK2/xjTVPCn91cEskZ8kyQ4IkPQTjm5/WntfCwbZauJQJKfGC4tCTTGzv83yDff/tB+07iSIQ==" saltValue="/KhouqfTR1M83iTX114muQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
-  <mergeCells count="4">
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="I10:K10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{23FE358A-EED1-43FA-B7B5-44EB7C7B3251}">
-          <x14:formula1>
-            <xm:f>Listes!$C$2:$C$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>I8</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCB943E-2788-419C-9C92-95BD0D524763}">
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:H16"/>
@@ -4643,7 +3869,7 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4657,18 +3883,18 @@
         <v>27</v>
       </c>
       <c r="D3">
-        <f>Magistrats!I4</f>
+        <f>'Calculatrice magistrats'!I4</f>
         <v>208</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="56">
+      <c r="F3" s="51">
         <f>D3</f>
         <v>208</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4688,7 +3914,7 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="55">
+      <c r="F4" s="50">
         <f>F3*2</f>
         <v>416</v>
       </c>
@@ -4698,7 +3924,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <f>1/Magistrats!I5</f>
+        <f>1/'Calculatrice magistrats'!I5</f>
         <v>0.125</v>
       </c>
       <c r="C5" t="s">
@@ -4710,7 +3936,7 @@
       <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="55">
+      <c r="F5" s="50">
         <f>D3*8</f>
         <v>1664</v>
       </c>
@@ -4732,11 +3958,11 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="33"/>
+      <c r="B9" s="32"/>
       <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="32"/>
       <c r="E9" t="s">
         <v>7</v>
       </c>
@@ -4745,21 +3971,21 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="33">
-        <f>Fonctionnaires!I5/5</f>
+      <c r="B10" s="32">
+        <f>'Calculatrice fonctionnaires'!I5/5</f>
         <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="33">
-        <f>Fonctionnaires!I4/Listes!B10</f>
+      <c r="D10" s="32">
+        <f>'Calculatrice fonctionnaires'!I4/Listes!B10</f>
         <v>229.57142857142858</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="56">
+      <c r="F10" s="51">
         <f>D10</f>
         <v>229.57142857142858</v>
       </c>
@@ -4768,21 +3994,21 @@
       <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="32">
         <f>B10/2</f>
         <v>3.5</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="33">
-        <f>Fonctionnaires!I4/Fonctionnaires!I5</f>
+      <c r="D11" s="32">
+        <f>'Calculatrice fonctionnaires'!I4/'Calculatrice fonctionnaires'!I5</f>
         <v>45.914285714285711</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="55">
+      <c r="F11" s="50">
         <f>F10*2</f>
         <v>459.14285714285717</v>
       </c>
@@ -4791,46 +4017,46 @@
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="32">
         <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="32">
         <f>12</f>
         <v>12</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="55">
+      <c r="F12" s="50">
         <f>D10*7</f>
         <v>1607</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="B13" s="33"/>
+      <c r="B13" s="32"/>
       <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="36" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="36" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update automation fiche agent calculatrice
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -8,7 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7966841A-CC70-7B43-ACC3-AC5CB48230E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A65A4A-4CED-EA40-9128-96FFD9BA91DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="dAFiNLtSQoZPzUqdToTXKs4qYdfbVNd/wXNYOIhJavkOrovrw5BoPQ0qeOxkvrIO42rTGOmJWYluvdRkpWME3g==" workbookSaltValue="cJrfxJd+x4HYx9OL+ePFng==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
@@ -987,6 +988,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1046,9 +1050,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2869,12 +2870,12 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="86"/>
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="102" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="102"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="103"/>
       <c r="F6" s="43" t="s">
         <v>79</v>
       </c>
@@ -2900,8 +2901,8 @@
       <c r="B8" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="104"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="105"/>
       <c r="E8" s="94" t="s">
         <v>75</v>
       </c>
@@ -2936,7 +2937,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="H4fmSqK3sKXM7B81Wq8se2UT5ifomk34hHyqjjl62dMlHzXYXc7kMPrFuAZvmQ1x6yaH2gGEwe7TtEUCMqrX1w==" saltValue="p2edxMsUn9E0W3EDH9+3fw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="PovsjZ3fs6fg8Fjg2GS3pw9Iq+QOC91oLp3ic3BMQIkQybreI0izcNbq15L5Gs3gNuEXQVrYIMG7Opm18YQJRA==" saltValue="vNwRWTFN4eLTX9JEiz4MQQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="2">
     <mergeCell ref="B6:E6"/>
@@ -3037,7 +3038,9 @@
     <col min="13" max="13" width="19.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="68" customHeight="1" thickBot="1"/>
+    <row r="1" spans="2:13" ht="68" customHeight="1" thickBot="1">
+      <c r="M1" s="13"/>
+    </row>
     <row r="2" spans="2:13" ht="6" customHeight="1">
       <c r="B2" s="19"/>
       <c r="C2" s="4"/>
@@ -3049,14 +3052,13 @@
       <c r="J2" s="61"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
-      <c r="M2"/>
     </row>
     <row r="3" spans="2:13" ht="40.5" customHeight="1">
       <c r="B3" s="27" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="99"/>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="101" t="s">
         <v>85</v>
       </c>
       <c r="E3" s="98"/>
@@ -3075,10 +3077,10 @@
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="26"/>
-      <c r="G4" s="110" t="s">
+      <c r="G4" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="111"/>
+      <c r="H4" s="112"/>
       <c r="I4" s="54"/>
       <c r="J4" s="2">
         <v>208</v>
@@ -3089,10 +3091,10 @@
       </c>
     </row>
     <row r="5" spans="2:13" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1">
-      <c r="G5" s="112" t="s">
+      <c r="G5" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="113"/>
+      <c r="H5" s="114"/>
       <c r="I5" s="55"/>
       <c r="J5" s="6">
         <v>8</v>
@@ -3108,7 +3110,7 @@
       <c r="I6" s="33"/>
     </row>
     <row r="7" spans="2:13" ht="70" customHeight="1">
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="109" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
@@ -3116,21 +3118,21 @@
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
-      <c r="F7" s="107" t="s">
+      <c r="F7" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="107"/>
+      <c r="G7" s="108"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="105" t="s">
+      <c r="J7" s="106" t="s">
         <v>20</v>
       </c>
       <c r="K7" s="52"/>
       <c r="M7"/>
     </row>
     <row r="8" spans="2:13" ht="26" customHeight="1">
-      <c r="B8" s="109"/>
-      <c r="J8" s="106"/>
+      <c r="B8" s="110"/>
+      <c r="J8" s="107"/>
       <c r="K8" s="53"/>
       <c r="M8"/>
     </row>
@@ -3150,7 +3152,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="63" t="str">
-        <f>IF($C$3="","",(C9*(VLOOKUP(F9,Listes!$A$2:$B$5,2,FALSE))*VLOOKUP(G9,Listes!$C$2:$D$6,2,FALSE))/($J$4*$C$3))</f>
+        <f>IF($C$3="","",(C9*(VLOOKUP(F9,Listes!$A$2:$B$5,2,FALSE))*VLOOKUP(G9,Listes!$C$2:$D$6,2,FALSE))/($J$4*($C$3/100)))</f>
         <v/>
       </c>
       <c r="K9" s="59"/>
@@ -3174,7 +3176,7 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="2:13" ht="69" customHeight="1">
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="109" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="31" t="s">
@@ -3191,12 +3193,12 @@
       <c r="M12"/>
     </row>
     <row r="13" spans="2:13" ht="34.5" customHeight="1">
-      <c r="B13" s="109"/>
+      <c r="B13" s="110"/>
       <c r="C13" s="60"/>
       <c r="D13" s="60"/>
       <c r="E13" s="60"/>
       <c r="F13" s="56"/>
-      <c r="H13" s="106" t="s">
+      <c r="H13" s="107" t="s">
         <v>21</v>
       </c>
       <c r="I13" s="53"/>
@@ -3212,7 +3214,7 @@
       <c r="F14" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="106"/>
+      <c r="H14" s="107"/>
       <c r="I14" s="53"/>
       <c r="J14" s="10"/>
     </row>
@@ -3237,7 +3239,7 @@
         <v>6</v>
       </c>
       <c r="H16" s="63" t="str">
-        <f>IF($C$3="","",(C14*VLOOKUP(F14,Listes!A2:B5,2,FALSE))*C16*VLOOKUP(F16,Listes!C2:D6,2,FALSE)/($J$4*$C$3))</f>
+        <f>IF($C$3="","",(C14*VLOOKUP(F14,Listes!A2:B5,2,FALSE))*C16*VLOOKUP(F16,Listes!C2:D6,2,FALSE)/($J$4*($C$3/100)))</f>
         <v/>
       </c>
       <c r="I16" s="22"/>
@@ -3269,7 +3271,7 @@
       <c r="E19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="XyY0EzQSHwdRLZ0/qTTDJnzh9WjI0LFcSk799vr9Ub8y0xTQx/jTqzgg59NWHos/thW1Xa18uN8XgxNlmlYtSQ==" saltValue="LZXV/F3pDhM8+VbdCrfdgg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="hxoMk4L3/LisHNG4Z9lcj8iUHZ2STxCDjyVpxNe6RPK3zdUxEowuwfDm7OxF+TTAB49/4e+wdhEKauLCGTvdFQ==" saltValue="PRrS+nfR6sokcupA5WblZQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="F7:G7"/>
@@ -3348,18 +3350,18 @@
         <v>24</v>
       </c>
       <c r="C3" s="99"/>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="101" t="s">
         <v>85</v>
       </c>
       <c r="E3" s="98"/>
-      <c r="G3" s="114" t="s">
+      <c r="G3" s="115" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="117"/>
       <c r="M3"/>
     </row>
     <row r="4" spans="2:13" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
@@ -3369,10 +3371,10 @@
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="26"/>
-      <c r="G4" s="110" t="s">
+      <c r="G4" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="111"/>
+      <c r="H4" s="112"/>
       <c r="I4" s="54"/>
       <c r="J4" s="10">
         <v>1607</v>
@@ -3383,10 +3385,10 @@
       </c>
     </row>
     <row r="5" spans="2:13" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="G5" s="112" t="s">
+      <c r="G5" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="113"/>
+      <c r="H5" s="114"/>
       <c r="I5" s="55"/>
       <c r="J5" s="100">
         <v>35</v>
@@ -3403,7 +3405,7 @@
       </c>
     </row>
     <row r="7" spans="2:13" ht="70" customHeight="1">
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="109" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
@@ -3411,21 +3413,21 @@
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
-      <c r="F7" s="107" t="s">
+      <c r="F7" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="107"/>
+      <c r="G7" s="108"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="105" t="s">
+      <c r="J7" s="106" t="s">
         <v>20</v>
       </c>
       <c r="K7" s="52"/>
       <c r="M7"/>
     </row>
     <row r="8" spans="2:13" ht="26" customHeight="1">
-      <c r="B8" s="109"/>
-      <c r="J8" s="106"/>
+      <c r="B8" s="110"/>
+      <c r="J8" s="107"/>
       <c r="K8" s="53"/>
       <c r="M8"/>
     </row>
@@ -3444,7 +3446,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="63" t="str">
-        <f>IF($C$3="","",(C9*(VLOOKUP(F9,Listes!$A$9:$B$12,2,FALSE))*VLOOKUP(G9,Listes!$C$9:$D$13,2,FALSE))/(($J$4)*$C$3))</f>
+        <f>IF($C$3="","",(C9*(VLOOKUP(F9,Listes!$A$9:$B$12,2,FALSE))*VLOOKUP(G9,Listes!$C$9:$D$13,2,FALSE))/(($J$4)*($C$3/100)))</f>
         <v/>
       </c>
       <c r="K9" s="22"/>
@@ -3470,7 +3472,7 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="2:13" ht="69" customHeight="1">
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="109" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="83" t="s">
@@ -3487,12 +3489,12 @@
       <c r="M12"/>
     </row>
     <row r="13" spans="2:13" ht="34.5" customHeight="1">
-      <c r="B13" s="109"/>
+      <c r="B13" s="110"/>
       <c r="C13" s="84"/>
       <c r="D13" s="84"/>
       <c r="E13" s="60"/>
       <c r="F13" s="56"/>
-      <c r="H13" s="106" t="s">
+      <c r="H13" s="107" t="s">
         <v>21</v>
       </c>
       <c r="I13" s="53"/>
@@ -3508,7 +3510,7 @@
       <c r="F14" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="106"/>
+      <c r="H14" s="107"/>
       <c r="I14" s="53"/>
       <c r="J14" s="10"/>
     </row>
@@ -3533,7 +3535,7 @@
         <v>6</v>
       </c>
       <c r="H16" s="65" t="str">
-        <f>IF($C$3="","",(C14*VLOOKUP(F14,Listes!A9:B12,2,FALSE))*C16*VLOOKUP(F16,Listes!C9:D13,2,FALSE)/($J$4*$C$3))</f>
+        <f>IF($C$3="","",(C14*VLOOKUP(F14,Listes!A9:B12,2,FALSE))*C16*VLOOKUP(F16,Listes!C9:D13,2,FALSE)/($J$4*($C$3/100)))</f>
         <v/>
       </c>
       <c r="I16" s="22"/>
@@ -3565,7 +3567,7 @@
       <c r="E19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DYZ3FFJLudNtb4awxuaxmNhFKrgigwJl67EfYFw2PWLs1cEmxsgQapSbo91YMrnfTw0gsfdtfYp29de4PrRxWw==" saltValue="zDF1EuQDBuY7aaVwhLnzmg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xWFdRrgTdcspR77r2V/831NLY2XiqfR7d2rnxi1SD1tWSHANkAJ2nhdOg07QhkLzwhubkN+8zMuvTJHpWvzF3Q==" saltValue="hMWHATj0PBbB9G4tZEvn/A==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="8">
     <mergeCell ref="G3:L3"/>
     <mergeCell ref="J7:J8"/>
@@ -3605,7 +3607,7 @@
   <dimension ref="C1:I22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="24" customHeight="1"/>
@@ -3628,30 +3630,30 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="3:9" ht="54.75" customHeight="1">
-      <c r="C2" s="118" t="s">
+      <c r="C2" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
     </row>
     <row r="3" spans="3:9" ht="27.75" customHeight="1">
       <c r="C3" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="117" t="s">
+      <c r="D3" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="117"/>
-      <c r="F3" s="119" t="s">
+      <c r="E3" s="118"/>
+      <c r="F3" s="120" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
     </row>
     <row r="4" spans="3:9" ht="23.25" customHeight="1">
       <c r="C4" s="38" t="s">
@@ -3881,7 +3883,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H1:H17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4094,6 +4096,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="VeIioI6SlBkZ5/EVBGW5gIzAzZjJEESwBC3xZ2mQulXnUIOMYkx8KPo8luI2ZBKG4IhsjhN79dp2coSu48OBfA==" saltValue="N9TCOS47uVRAid0CA0wpmw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update message erreur fiche de temps
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A65A4A-4CED-EA40-9128-96FFD9BA91DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29445E58-9B73-294B-A5C0-764931035A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="dAFiNLtSQoZPzUqdToTXKs4qYdfbVNd/wXNYOIhJavkOrovrw5BoPQ0qeOxkvrIO42rTGOmJWYluvdRkpWME3g==" workbookSaltValue="cJrfxJd+x4HYx9OL+ePFng==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
@@ -2937,7 +2937,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="PovsjZ3fs6fg8Fjg2GS3pw9Iq+QOC91oLp3ic3BMQIkQybreI0izcNbq15L5Gs3gNuEXQVrYIMG7Opm18YQJRA==" saltValue="vNwRWTFN4eLTX9JEiz4MQQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="fAwv5b7PhGyp8Uus7PUXl6MY7tUE+6QZrnFNDXOa/NDQH5sGFC9l2az0xhi1ZHK/s+UhfsUabhdd/ho885ShYQ==" saltValue="2h+f5XD5gSzjicnGkgPLPw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="2">
     <mergeCell ref="B6:E6"/>
@@ -2978,7 +2978,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{36A38D39-CE0C-451A-AF08-7EA966C140A2}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alerte saisie !" error="Pour ce contentieux, il est nécessaire de détailler les sous contentieux figurant sur fond jaune. Cliquez sur &quot;Annuler&quot; et saisissez le détail indiqué précédement. Le total se calcule automatiquement." sqref="E9:E300" xr:uid="{E57D8FC0-574C-314A-A32B-42F38B89AA92}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alerte saisie !" error="Pour ce contentieux, il est nécessaire de détailler les sous-contentieux. Cliquez sur “Annuler” et renseignez le pourcentage d’ETPT correspondant aux sous-contentieux figurant en jaune. Le total du contentieux se calculera automatiquement." sqref="E10:E300" xr:uid="{18B294E4-7153-4D4A-A339-C814EBC12311}">
       <formula1>AND($B10&lt;&gt;"TOTAL Juges des Enfants",$B10&lt;&gt;"TOTAL Juges d'Instruction",$B10&lt;&gt;"TOTAL Contentieux des mineurs")</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update fiche agent bloquage autres act
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29445E58-9B73-294B-A5C0-764931035A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E64BE86-5144-E248-BE2F-3537F77346A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="dAFiNLtSQoZPzUqdToTXKs4qYdfbVNd/wXNYOIhJavkOrovrw5BoPQ0qeOxkvrIO42rTGOmJWYluvdRkpWME3g==" workbookSaltValue="cJrfxJd+x4HYx9OL+ePFng==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
@@ -2937,7 +2937,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="fAwv5b7PhGyp8Uus7PUXl6MY7tUE+6QZrnFNDXOa/NDQH5sGFC9l2az0xhi1ZHK/s+UhfsUabhdd/ho885ShYQ==" saltValue="2h+f5XD5gSzjicnGkgPLPw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="OA+22Pp7aTOvCRx0g6GY4Xhng7YWimRDbIRuBiIXhAsutSZxCbM14zShI8KOToQG2pGXQuYUmpzZwMGFr3nobQ==" saltValue="IWZ5lfVCc9KftHvtGHAAyA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="2">
     <mergeCell ref="B6:E6"/>
@@ -2979,7 +2979,7 @@
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alerte saisie !" error="Pour ce contentieux, il est nécessaire de détailler les sous-contentieux. Cliquez sur “Annuler” et renseignez le pourcentage d’ETPT correspondant aux sous-contentieux figurant en jaune. Le total du contentieux se calculera automatiquement." sqref="E10:E300" xr:uid="{18B294E4-7153-4D4A-A339-C814EBC12311}">
-      <formula1>AND($B10&lt;&gt;"TOTAL Juges des Enfants",$B10&lt;&gt;"TOTAL Juges d'Instruction",$B10&lt;&gt;"TOTAL Contentieux des mineurs")</formula1>
+      <formula1>AND($B10&lt;&gt;"TOTAL Juges des Enfants",$B10&lt;&gt;"TOTAL Juges d'Instruction",$B10&lt;&gt;"TOTAL Contentieux des mineurs",$B10&lt;&gt;"TOTAL Autres activités")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add fiche de temps date info
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD77926E-BD33-CF41-A47C-5BAA02FE65A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5B2AF5-26B4-324F-A558-6228C7F0A140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="dAFiNLtSQoZPzUqdToTXKs4qYdfbVNd/wXNYOIhJavkOrovrw5BoPQ0qeOxkvrIO42rTGOmJWYluvdRkpWME3g==" workbookSaltValue="cJrfxJd+x4HYx9OL+ePFng==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15760" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille de temps" sheetId="8" r:id="rId1"/>
@@ -2937,7 +2937,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="OA+22Pp7aTOvCRx0g6GY4Xhng7YWimRDbIRuBiIXhAsutSZxCbM14zShI8KOToQG2pGXQuYUmpzZwMGFr3nobQ==" saltValue="IWZ5lfVCc9KftHvtGHAAyA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="F/1XwNDctTMjAe1UqFyOU3aCv+gnRaZPGHwcmL4SqknvWQaPI/7IkesRGUX30phf49q7Kf0kEmrHwu9T0bsgDA==" saltValue="xU3uwDSh22o4BWRy3BtdsA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="2">
     <mergeCell ref="B6:E6"/>
@@ -2972,15 +2972,13 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Erreur de saisie" error="Vous devez choisir une fonction dans la liste proposée !" sqref="C4" xr:uid="{4B86F8E2-A2C1-4AF0-8AD2-6F6FB121C7E1}">
       <formula1>INDIRECT(SUBSTITUTE($C$2," ","_"))</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date non valide" error="Saisir une date au format JJ/MM/AAAA" sqref="C8" xr:uid="{A91592D5-FAF1-48BE-B5FE-60B612F0C2AB}">
-      <formula1>1</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{36A38D39-CE0C-451A-AF08-7EA966C140A2}">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alerte saisie !" error="Pour ce contentieux, il est nécessaire de détailler les sous-contentieux. Cliquez sur “Annuler” et renseignez le pourcentage d’ETPT correspondant aux sous-contentieux figurant en jaune. Le total du contentieux se calculera automatiquement." sqref="E10:E300" xr:uid="{18B294E4-7153-4D4A-A339-C814EBC12311}">
       <formula1>AND($B10&lt;&gt;"TOTAL Juges des Enfants",$B10&lt;&gt;"TOTAL Juges d'Instruction",$B10&lt;&gt;"TOTAL Contentieux des mineurs",$B10&lt;&gt;"TOTAL Autres activités")</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Saisir une date" prompt="Afin que la date soit validée, merci de la saisir au format JJ/MM/AAAA." sqref="C8:D8" xr:uid="{8ABA325E-5DD9-AE4F-8441-E40828C3610A}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
update fiche de temps
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5B2AF5-26B4-324F-A558-6228C7F0A140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD6D42C-51F2-4341-9340-92B66246DDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="dAFiNLtSQoZPzUqdToTXKs4qYdfbVNd/wXNYOIhJavkOrovrw5BoPQ0qeOxkvrIO42rTGOmJWYluvdRkpWME3g==" workbookSaltValue="cJrfxJd+x4HYx9OL+ePFng==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15760" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
@@ -2937,7 +2937,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="F/1XwNDctTMjAe1UqFyOU3aCv+gnRaZPGHwcmL4SqknvWQaPI/7IkesRGUX30phf49q7Kf0kEmrHwu9T0bsgDA==" saltValue="xU3uwDSh22o4BWRy3BtdsA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="YDLMdyimdH9HolrCjOWAmESRcQtly2SSciKvfMbDn1ll0ROvvxVLaguVmB2dPeyLFUiHYbuzjlRWeim82//lyg==" saltValue="5lC+JKUWtcx2wFxIpMpnuQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="2">
     <mergeCell ref="B6:E6"/>
@@ -2970,7 +2970,7 @@
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Erreur de saisie" error="Vous devez choisir une fonction dans la liste proposée !" sqref="C4" xr:uid="{4B86F8E2-A2C1-4AF0-8AD2-6F6FB121C7E1}">
-      <formula1>INDIRECT(SUBSTITUTE($C$2," ","_"))</formula1>
+      <formula1>OFFSET(INDIRECT(SUBSTITUTE($C$2," ","_")),0,0,COUNTA(INDIRECT(SUBSTITUTE($C$2," ","_"))),1)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{36A38D39-CE0C-451A-AF08-7EA966C140A2}">
       <formula1>#REF!</formula1>
@@ -3016,7 +3016,7 @@
   <dimension ref="B1:M19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3269,7 +3269,7 @@
       <c r="E19" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="LVLIzFqr3WSYpyM6mAPeDH5PbVQuovQ7oA15kWks36OjNp987cHOlor2LHQ19fkTDK14zjYb75JwlwUNhRJeJQ==" saltValue="/5PvXz7PMWKVm++AO7LsOQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="bmsqbZxTbIWnjlHD//PIizDMMZ4611sv4dJDqBJg0v7s2baPDSyZeppLMDHrL5Ojd8NKJ1l/LpqudGYKGJq2hA==" saltValue="WOHHcsfRGK3z/SF+Zfd6Uw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="F7:G7"/>

</xml_diff>

<commit_message>
export current situation to excel
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francois-xaviermontigny/git/beta.gouv.fr/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD6D42C-51F2-4341-9340-92B66246DDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EC39C8-35F7-FE42-9901-9DA881529767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="dAFiNLtSQoZPzUqdToTXKs4qYdfbVNd/wXNYOIhJavkOrovrw5BoPQ0qeOxkvrIO42rTGOmJWYluvdRkpWME3g==" workbookSaltValue="cJrfxJd+x4HYx9OL+ePFng==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15760" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
+    <workbookView xWindow="-27200" yWindow="620" windowWidth="27040" windowHeight="15760" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille de temps" sheetId="8" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
   <si>
     <t>Temps de travail d'un magistrat</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>## c.value</t>
   </si>
 </sst>
 </file>
@@ -2795,7 +2798,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="110" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2921,7 +2924,9 @@
         <v>81</v>
       </c>
       <c r="D9" s="96"/>
-      <c r="E9" s="97"/>
+      <c r="E9" s="97" t="s">
+        <v>86</v>
+      </c>
       <c r="F9" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
update time file with 2 decimals
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francois-xaviermontigny/git/beta.gouv.fr/a-just/front/src/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EC39C8-35F7-FE42-9901-9DA881529767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2849719-7F07-F548-B78F-74B78CE15F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="dAFiNLtSQoZPzUqdToTXKs4qYdfbVNd/wXNYOIhJavkOrovrw5BoPQ0qeOxkvrIO42rTGOmJWYluvdRkpWME3g==" workbookSaltValue="cJrfxJd+x4HYx9OL+ePFng==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-27200" yWindow="620" windowWidth="27040" windowHeight="15760" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15860" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille de temps" sheetId="8" r:id="rId1"/>
@@ -965,9 +965,6 @@
     <xf numFmtId="4" fontId="13" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -993,6 +990,9 @@
     </xf>
     <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2798,7 +2798,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="110" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2894,7 +2894,7 @@
       <c r="D7" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="93"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="43" t="s">
         <v>79</v>
       </c>
@@ -2906,7 +2906,7 @@
       </c>
       <c r="C8" s="104"/>
       <c r="D8" s="105"/>
-      <c r="E8" s="94" t="s">
+      <c r="E8" s="93" t="s">
         <v>75</v>
       </c>
       <c r="F8" t="s">
@@ -2917,14 +2917,14 @@
       <c r="A9" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="96" t="s">
+      <c r="C9" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="96"/>
-      <c r="E9" s="97" t="s">
+      <c r="D9" s="95"/>
+      <c r="E9" s="96" t="s">
         <v>86</v>
       </c>
       <c r="F9" t="s">
@@ -2942,7 +2942,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="YDLMdyimdH9HolrCjOWAmESRcQtly2SSciKvfMbDn1ll0ROvvxVLaguVmB2dPeyLFUiHYbuzjlRWeim82//lyg==" saltValue="5lC+JKUWtcx2wFxIpMpnuQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="pgQS/rT3LSns4KzWNXcQ9XcGBB1gibieups544Fhyq9b+u+01iguPkuvhiuqqGvnJ9QSYfLwfJSVEOWNpOkCUA==" saltValue="hfcqhFB1qRDzRVXnLcBmiw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="2">
     <mergeCell ref="B6:E6"/>
@@ -3060,11 +3060,11 @@
       <c r="B3" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="101" t="s">
+      <c r="C3" s="98"/>
+      <c r="D3" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="98"/>
+      <c r="E3" s="97"/>
       <c r="G3" s="18" t="s">
         <v>19</v>
       </c>
@@ -3352,11 +3352,11 @@
       <c r="B3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="101" t="s">
+      <c r="C3" s="98"/>
+      <c r="D3" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="98"/>
+      <c r="E3" s="97"/>
       <c r="G3" s="115" t="s">
         <v>37</v>
       </c>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="H5" s="114"/>
       <c r="I5" s="55"/>
-      <c r="J5" s="100">
+      <c r="J5" s="99">
         <v>35</v>
       </c>
       <c r="K5" s="35"/>

</xml_diff>